<commit_message>
sexy excelhandler daniels har nogle fjong finurlige jader og han ved det
</commit_message>
<xml_diff>
--- a/slayysaft.xlsx
+++ b/slayysaft.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\programmering\MaltMadness\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olive\Desktop\Programmering\MaltMadness\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7746CF44-806F-4C77-9E93-75B7638220C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E5F9D5-CB06-4622-AB92-F73687BE7BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10" yWindow="10" windowWidth="22540" windowHeight="14300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hva" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>SPØRGSMÅL</t>
   </si>
@@ -59,6 +59,48 @@
   </si>
   <si>
     <t>ABSURD</t>
+  </si>
+  <si>
+    <t>Hvad fuck sker der her</t>
+  </si>
+  <si>
+    <t>Ingen ved det</t>
+  </si>
+  <si>
+    <t>Alle vil vide det</t>
+  </si>
+  <si>
+    <t>Find selv ud af det</t>
+  </si>
+  <si>
+    <t>Fire jo</t>
+  </si>
+  <si>
+    <t>Gustav er fuldstændig uden for pedagogisk rækkeviede?</t>
+  </si>
+  <si>
+    <t>Yeps</t>
+  </si>
+  <si>
+    <t>Joooeh</t>
+  </si>
+  <si>
+    <t>Helt 100</t>
+  </si>
+  <si>
+    <t>Selvfølgelig</t>
+  </si>
+  <si>
+    <t>Hvor meget vejer det tungeste gram?</t>
+  </si>
+  <si>
+    <t>Mindst 5 ihvertfald</t>
+  </si>
+  <si>
+    <t>måske et helt</t>
+  </si>
+  <si>
+    <t>omtrænt ligeså meget som min højre nos</t>
   </si>
 </sst>
 </file>
@@ -376,23 +418,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="56.77734375" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" customWidth="1"/>
-    <col min="3" max="3" width="21.88671875" customWidth="1"/>
-    <col min="4" max="4" width="22.44140625" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="56.81640625" customWidth="1"/>
+    <col min="2" max="2" width="24.54296875" customWidth="1"/>
+    <col min="3" max="3" width="21.90625" customWidth="1"/>
+    <col min="4" max="4" width="22.453125" customWidth="1"/>
+    <col min="5" max="5" width="38.7265625" customWidth="1"/>
+    <col min="6" max="6" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -412,7 +454,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -429,6 +471,66 @@
         <v>10</v>
       </c>
       <c r="F2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5">
         <v>4</v>
       </c>
     </row>
@@ -443,7 +545,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
susususuusususususuusus dani fucker med min hjerne
</commit_message>
<xml_diff>
--- a/slayysaft.xlsx
+++ b/slayysaft.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olive\Desktop\Programmering\MaltMadness\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E5F9D5-CB06-4622-AB92-F73687BE7BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792A047E-E916-422D-A9C1-FE6F7A9E9013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10" yWindow="10" windowWidth="22540" windowHeight="14300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10" yWindow="10" windowWidth="22540" windowHeight="14300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hva" sheetId="1" r:id="rId1"/>
     <sheet name="alko" sheetId="2" r:id="rId2"/>
+    <sheet name="sode" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>SPØRGSMÅL</t>
   </si>
@@ -101,14 +102,61 @@
   </si>
   <si>
     <t>omtrænt ligeså meget som min højre nos</t>
+  </si>
+  <si>
+    <t>Vodka</t>
+  </si>
+  <si>
+    <t>Gin</t>
+  </si>
+  <si>
+    <t>Alkohol</t>
+  </si>
+  <si>
+    <t>Opblanding</t>
+  </si>
+  <si>
+    <t>Applesinjuice</t>
+  </si>
+  <si>
+    <t>Kakao</t>
+  </si>
+  <si>
+    <t>Coca Cola</t>
+  </si>
+  <si>
+    <t>Gazoz</t>
+  </si>
+  <si>
+    <t>Rom</t>
+  </si>
+  <si>
+    <t>Hvidrom</t>
+  </si>
+  <si>
+    <t>Små Sure</t>
+  </si>
+  <si>
+    <t>Fanta</t>
+  </si>
+  <si>
+    <t>Tonic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -136,8 +184,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -541,12 +590,101 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4947EF9-1F32-4373-875C-0B469E94E8FE}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.36328125" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DE5E166-630D-446A-843C-8792D2283430}">
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ikke for folk med gigt da, (svage kællinger)
</commit_message>
<xml_diff>
--- a/slayysaft.xlsx
+++ b/slayysaft.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olive\Desktop\Programmering\MaltMadness\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3177EC-A53D-4A8F-BD1E-E706EA0A3E70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F49AA1B4-A73F-4AD9-8762-75905A060034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10" yWindow="10" windowWidth="22540" windowHeight="14300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
   <si>
     <t>SPØRGSMÅL</t>
   </si>
@@ -185,6 +185,18 @@
   </si>
   <si>
     <t>du er flink nok når du ikke snakker</t>
+  </si>
+  <si>
+    <t>hehehe prut</t>
+  </si>
+  <si>
+    <t>du er dum og grim</t>
+  </si>
+  <si>
+    <t>hej med dig</t>
+  </si>
+  <si>
+    <t>sån er det bare</t>
   </si>
 </sst>
 </file>
@@ -735,10 +747,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74498D84-E07C-43BD-86A1-84DD25E5001E}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -773,6 +785,38 @@
       </c>
       <c r="B4" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -785,7 +829,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
jaja det er flot ik
</commit_message>
<xml_diff>
--- a/slayysaft.xlsx
+++ b/slayysaft.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olive\Desktop\Programmering\MaltMadness\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D5F5EE8-601D-4E18-8E3A-3BF1D37C3026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E600C92-4D86-4C2F-B2AB-7E69B31B9298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hva" sheetId="1" r:id="rId1"/>
@@ -876,8 +876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1505,6 +1505,9 @@
       </c>
       <c r="E31" t="s">
         <v>168</v>
+      </c>
+      <c r="F31">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1696,7 +1699,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61F2349D-0664-4FC8-9C83-F9C5C9C53257}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>

</xml_diff>